<commit_message>
renamed columns and created FAT.ALL with merged yearly and monthly Data
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marvin\OneDrive\Desktop\Studium\SS21\Seminar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marvin\FAT-Seminar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E16575C9-6CB8-496B-908C-F5E8D91C5DFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE41810A-1A91-4BA7-BD14-70F3904C28AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C0A3B511-10A9-409F-B613-03E796592B5D}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{C0A3B511-10A9-409F-B613-03E796592B5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>06.05.2021-13.05.2021</t>
   </si>
@@ -91,6 +91,24 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t>Create hedge portfolio from factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 8 </t>
+  </si>
+  <si>
+    <t>Run CAPM regression on hedge portfolio to check for excess return</t>
+  </si>
+  <si>
+    <t>Task 9</t>
+  </si>
+  <si>
+    <t>Re-Create Table 3 and Table 4 from Hanauer, Lauterbach Paper</t>
   </si>
 </sst>
 </file>
@@ -442,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157C5407-56AD-4C61-97D8-5DA3DA00332C}">
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,6 +548,30 @@
         <v>12</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>